<commit_message>
Rediseno de GUI, con CustomTkinter, y reposicion de buttons
</commit_message>
<xml_diff>
--- a/clustersEmpleados.xlsx
+++ b/clustersEmpleados.xlsx
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -762,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -867,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="K20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="K22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1392,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
       <c r="K35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -1742,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="K39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1917,7 +1917,7 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -2337,7 +2337,7 @@
         <v>1</v>
       </c>
       <c r="K54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -2442,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="K62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="K63" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="K65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="K67" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
       <c r="K69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -2967,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="K72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
@@ -3037,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -3142,7 +3142,7 @@
         <v>0</v>
       </c>
       <c r="K77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -3177,7 +3177,7 @@
         <v>1</v>
       </c>
       <c r="K78" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="K80" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3317,7 +3317,7 @@
         <v>1</v>
       </c>
       <c r="K82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -3387,7 +3387,7 @@
         <v>1</v>
       </c>
       <c r="K84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -3492,7 +3492,7 @@
         <v>1</v>
       </c>
       <c r="K87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="K89" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90">
@@ -3667,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="K93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="K95" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
@@ -3842,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="K97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="K99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100">
@@ -4017,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="K102" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -4087,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="K104" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105">
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="K107" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -4227,7 +4227,7 @@
         <v>1</v>
       </c>
       <c r="K108" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
@@ -4297,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111">
@@ -4367,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="K112" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="K114" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
@@ -4542,7 +4542,7 @@
         <v>1</v>
       </c>
       <c r="K117" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
@@ -4612,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="K119" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120">
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="K122" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -4752,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="K123" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124">
@@ -4822,7 +4822,7 @@
         <v>1</v>
       </c>
       <c r="K125" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
@@ -4892,7 +4892,7 @@
         <v>1</v>
       </c>
       <c r="K127" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
@@ -4962,7 +4962,7 @@
         <v>1</v>
       </c>
       <c r="K129" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
@@ -5067,7 +5067,7 @@
         <v>1</v>
       </c>
       <c r="K132" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="K134" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135">
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="K137" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -5277,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="K138" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139">
@@ -5347,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="K140" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141">
@@ -5417,7 +5417,7 @@
         <v>1</v>
       </c>
       <c r="K142" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143">
@@ -5487,7 +5487,7 @@
         <v>1</v>
       </c>
       <c r="K144" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
@@ -5592,7 +5592,7 @@
         <v>1</v>
       </c>
       <c r="K147" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -5662,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="K149" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150">
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="K152" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -5802,7 +5802,7 @@
         <v>1</v>
       </c>
       <c r="K153" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
@@ -5872,7 +5872,7 @@
         <v>1</v>
       </c>
       <c r="K155" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156">
@@ -5942,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="K157" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
@@ -6012,7 +6012,7 @@
         <v>1</v>
       </c>
       <c r="K159" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
@@ -6117,7 +6117,7 @@
         <v>1</v>
       </c>
       <c r="K162" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163">
@@ -6187,7 +6187,7 @@
         <v>1</v>
       </c>
       <c r="K164" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
@@ -6292,7 +6292,7 @@
         <v>0</v>
       </c>
       <c r="K167" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -6327,7 +6327,7 @@
         <v>1</v>
       </c>
       <c r="K168" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169">
@@ -6397,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="K170" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
@@ -6467,7 +6467,7 @@
         <v>1</v>
       </c>
       <c r="K172" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173">
@@ -6537,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="K174" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175">
@@ -6642,7 +6642,7 @@
         <v>1</v>
       </c>
       <c r="K177" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178">
@@ -6712,7 +6712,7 @@
         <v>1</v>
       </c>
       <c r="K179" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180">
@@ -6817,7 +6817,7 @@
         <v>0</v>
       </c>
       <c r="K182" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -6852,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="K183" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
@@ -6922,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="K185" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186">
@@ -6992,7 +6992,7 @@
         <v>1</v>
       </c>
       <c r="K187" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
@@ -7062,7 +7062,7 @@
         <v>1</v>
       </c>
       <c r="K189" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
@@ -7167,7 +7167,7 @@
         <v>1</v>
       </c>
       <c r="K192" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
@@ -7237,7 +7237,7 @@
         <v>1</v>
       </c>
       <c r="K194" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
@@ -7342,7 +7342,7 @@
         <v>0</v>
       </c>
       <c r="K197" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="K198" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199">
@@ -7447,7 +7447,7 @@
         <v>1</v>
       </c>
       <c r="K200" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201">
@@ -7517,7 +7517,7 @@
         <v>1</v>
       </c>
       <c r="K202" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203">
@@ -7587,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="K204" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205">
@@ -7692,7 +7692,7 @@
         <v>1</v>
       </c>
       <c r="K207" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="208">
@@ -7762,7 +7762,7 @@
         <v>1</v>
       </c>
       <c r="K209" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210">
@@ -7867,7 +7867,7 @@
         <v>0</v>
       </c>
       <c r="K212" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -7902,7 +7902,7 @@
         <v>1</v>
       </c>
       <c r="K213" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214">
@@ -7972,7 +7972,7 @@
         <v>1</v>
       </c>
       <c r="K215" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216">
@@ -8042,7 +8042,7 @@
         <v>1</v>
       </c>
       <c r="K217" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218">
@@ -8112,7 +8112,7 @@
         <v>1</v>
       </c>
       <c r="K219" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
@@ -8217,7 +8217,7 @@
         <v>1</v>
       </c>
       <c r="K222" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223">
@@ -8287,7 +8287,7 @@
         <v>1</v>
       </c>
       <c r="K224" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225">
@@ -8392,7 +8392,7 @@
         <v>0</v>
       </c>
       <c r="K227" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -8427,7 +8427,7 @@
         <v>1</v>
       </c>
       <c r="K228" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="229">
@@ -8497,7 +8497,7 @@
         <v>1</v>
       </c>
       <c r="K230" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231">
@@ -8567,7 +8567,7 @@
         <v>1</v>
       </c>
       <c r="K232" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233">
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="K234" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235">
@@ -8742,7 +8742,7 @@
         <v>1</v>
       </c>
       <c r="K237" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238">
@@ -8812,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="K239" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="240">
@@ -8917,7 +8917,7 @@
         <v>0</v>
       </c>
       <c r="K242" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -8952,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="K243" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244">
@@ -9022,7 +9022,7 @@
         <v>1</v>
       </c>
       <c r="K245" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="246">
@@ -9092,7 +9092,7 @@
         <v>1</v>
       </c>
       <c r="K247" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248">
@@ -9162,7 +9162,7 @@
         <v>1</v>
       </c>
       <c r="K249" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
@@ -9267,7 +9267,7 @@
         <v>1</v>
       </c>
       <c r="K252" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253">
@@ -9337,7 +9337,7 @@
         <v>1</v>
       </c>
       <c r="K254" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="255">
@@ -9442,7 +9442,7 @@
         <v>0</v>
       </c>
       <c r="K257" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -9477,7 +9477,7 @@
         <v>1</v>
       </c>
       <c r="K258" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259">
@@ -9547,7 +9547,7 @@
         <v>1</v>
       </c>
       <c r="K260" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261">
@@ -9617,7 +9617,7 @@
         <v>1</v>
       </c>
       <c r="K262" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263">
@@ -9687,7 +9687,7 @@
         <v>1</v>
       </c>
       <c r="K264" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265">
@@ -9792,7 +9792,7 @@
         <v>1</v>
       </c>
       <c r="K267" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268">
@@ -9862,7 +9862,7 @@
         <v>1</v>
       </c>
       <c r="K269" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="270">

</xml_diff>